<commit_message>
Finalize SQ1: Refined Parse Error Metrics (Empty/Label/Syntax), Fixed Group A Reporting, and 14B/32B Plot Support
</commit_message>
<xml_diff>
--- a/examples/single_agent/analysis/SQ1_Final_Results/sq1_metrics_rules.xlsx
+++ b/examples/single_agent/analysis/SQ1_Final_Results/sq1_metrics_rules.xlsx
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -593,16 +593,16 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>436</v>
+        <v>447</v>
       </c>
       <c r="K3">
         <v>160</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>59.96</v>
@@ -640,16 +640,16 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="K4">
         <v>146</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <v>58.77</v>
@@ -687,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -716,7 +716,7 @@
         <v>989</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -734,13 +734,13 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="K6">
         <v>26</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -810,7 +810,7 @@
         <v>886</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -828,7 +828,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K8">
         <v>3</v>
@@ -857,7 +857,7 @@
         <v>897</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -922,7 +922,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="K10">
         <v>0</v>

</xml_diff>

<commit_message>
chore: update experiment configs, analysis scripts, and add CLI hooks
- agent_types.yaml: updated governance rules and sampling defaults
- run_flood.py: improved CLI argument handling
- analysis scripts: corrected entropy audit, adaptation matrix
- archive/deepseek_r1_finished/: DeepSeek analysis scripts
- hooks/: UserPromptSubmit hook for codex-edit/gemini-edit delegation
- config/prompts/household.txt: externalized prompt template

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/examples/single_agent/analysis/SQ1_Final_Results/sq1_metrics_rules.xlsx
+++ b/examples/single_agent/analysis/SQ1_Final_Results/sq1_metrics_rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Model</t>
   </si>
@@ -61,16 +61,13 @@
     <t>Audit_Str</t>
   </si>
   <si>
-    <t>deepseek_r1_1_5b</t>
-  </si>
-  <si>
-    <t>deepseek_r1_8b</t>
-  </si>
-  <si>
-    <t>deepseek_r1_14b</t>
-  </si>
-  <si>
-    <t>deepseek_r1_32b</t>
+    <t>gemma3_4b</t>
+  </si>
+  <si>
+    <t>gemma3_12b</t>
+  </si>
+  <si>
+    <t>gemma3_27b</t>
   </si>
   <si>
     <t>Group_A</t>
@@ -82,34 +79,22 @@
     <t>Group_C</t>
   </si>
   <si>
-    <t>80|20</t>
-  </si>
-  <si>
-    <t>52|27</t>
-  </si>
-  <si>
-    <t>60|27</t>
-  </si>
-  <si>
-    <t>11|3</t>
-  </si>
-  <si>
-    <t>0|2</t>
+    <t>1|0</t>
+  </si>
+  <si>
+    <t>1|32</t>
+  </si>
+  <si>
+    <t>0|43</t>
+  </si>
+  <si>
+    <t>0|1</t>
+  </si>
+  <si>
+    <t>2|4</t>
   </si>
   <si>
     <t>0|0</t>
-  </si>
-  <si>
-    <t>68|10</t>
-  </si>
-  <si>
-    <t>4|29</t>
-  </si>
-  <si>
-    <t>5|31</t>
-  </si>
-  <si>
-    <t>24|11</t>
   </si>
 </sst>
 </file>
@@ -467,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -525,22 +510,22 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2">
-        <v>237</v>
+        <v>998</v>
       </c>
       <c r="D2">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="G2">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -549,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -561,10 +546,10 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>55.47</v>
+        <v>14.14</v>
       </c>
       <c r="O2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -572,46 +557,46 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>557</v>
+        <v>827</v>
       </c>
       <c r="D3">
-        <v>263</v>
+        <v>42</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>179</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>447</v>
+        <v>141</v>
       </c>
       <c r="K3">
-        <v>160</v>
+        <v>42</v>
       </c>
       <c r="L3">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>59.96</v>
+        <v>39.61</v>
       </c>
       <c r="O3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -619,46 +604,46 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>539</v>
+        <v>843</v>
       </c>
       <c r="D4">
-        <v>208</v>
+        <v>53</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>192</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>400</v>
+        <v>168</v>
       </c>
       <c r="K4">
-        <v>146</v>
+        <v>53</v>
       </c>
       <c r="L4">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>58.77</v>
+        <v>37.42</v>
       </c>
       <c r="O4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -666,22 +651,22 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>966</v>
+        <v>999</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -690,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -702,10 +687,10 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>17.21</v>
+        <v>17.58</v>
       </c>
       <c r="O5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -713,281 +698,93 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>989</v>
+        <v>969</v>
       </c>
       <c r="D6">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="K6">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="L6">
-        <v>163</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>44.54</v>
+        <v>24.86</v>
       </c>
       <c r="O6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>1000</v>
       </c>
       <c r="D7">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H7">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="K7">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>39.78</v>
+        <v>32.67</v>
       </c>
       <c r="O7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>728</v>
-      </c>
-      <c r="D8">
-        <v>68</v>
-      </c>
-      <c r="E8">
-        <v>68</v>
-      </c>
-      <c r="F8">
-        <v>78</v>
-      </c>
-      <c r="G8">
-        <v>78</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>146</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>24.52</v>
-      </c>
-      <c r="O8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9">
-        <v>886</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>9</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>42.24</v>
-      </c>
-      <c r="O9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>897</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>49.81</v>
-      </c>
-      <c r="O10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>916</v>
-      </c>
-      <c r="D11">
-        <v>24</v>
-      </c>
-      <c r="E11">
-        <v>24</v>
-      </c>
-      <c r="F11">
-        <v>85</v>
-      </c>
-      <c r="G11">
-        <v>85</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>109</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>27.08</v>
-      </c>
-      <c r="O11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>